<commit_message>
Changed group to batch
</commit_message>
<xml_diff>
--- a/xls/QA - 1 Easy.xlsx
+++ b/xls/QA - 1 Easy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>Question</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>half the data gets corrupted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>While working on a product if there are any open circuits which of the following signs would you use</t>
@@ -806,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -839,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>3</v>
@@ -1364,7 +1361,7 @@
         <v>101</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1372,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4">
@@ -1382,29 +1379,17 @@
         <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>